<commit_message>
[AOS] Test Result UI 작업
</commit_message>
<xml_diff>
--- a/Localization/LanguagePack.xlsx
+++ b/Localization/LanguagePack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimkihoon/Work/Project/EverydayJapanese/Localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CC4B9B-465F-2742-9169-085551460C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DE07F6-8DE1-524D-91EA-DF612328C17A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="760" windowWidth="33600" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="191">
   <si>
     <t>String_Index</t>
   </si>
@@ -674,6 +674,22 @@
   </si>
   <si>
     <t>테스트 끝내기</t>
+  </si>
+  <si>
+    <t>Core</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>틀린단어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>incorrect word</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>incorrect_word</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -789,7 +805,7 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1980,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F244"/>
+  <dimension ref="A1:F246"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2360,7 +2376,7 @@
       </c>
       <c r="B31" s="10"/>
       <c r="C31" s="9" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="D31" s="10"/>
     </row>
@@ -2769,58 +2785,68 @@
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="D66" s="12" t="s">
-        <v>180</v>
-      </c>
+      <c r="A66" s="6"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>183</v>
-      </c>
+      <c r="A67" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="10"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="12" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B68" s="12"/>
       <c r="C68" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="D69" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D68" s="12" t="s">
+      <c r="D70" s="12" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="6"/>
+    <row r="71" spans="1:4" ht="16">
+      <c r="A71" s="6" t="s">
+        <v>190</v>
+      </c>
       <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
+      <c r="C71" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="6"/>
@@ -3859,6 +3885,18 @@
       <c r="B244" s="6"/>
       <c r="C244" s="6"/>
       <c r="D244" s="6"/>
+    </row>
+    <row r="245" spans="1:4">
+      <c r="A245" s="6"/>
+      <c r="B245" s="6"/>
+      <c r="C245" s="6"/>
+      <c r="D245" s="6"/>
+    </row>
+    <row r="246" spans="1:4">
+      <c r="A246" s="6"/>
+      <c r="B246" s="6"/>
+      <c r="C246" s="6"/>
+      <c r="D246" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>